<commit_message>
fixed UI of all mails
</commit_message>
<xml_diff>
--- a/Download - All Mail.xlsx
+++ b/Download - All Mail.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="37">
   <si>
     <t>S.No</t>
   </si>
@@ -98,6 +98,30 @@
   </si>
   <si>
     <t>Test-Check-23</t>
+  </si>
+  <si>
+    <t>Veer_New-01</t>
+  </si>
+  <si>
+    <t>Test-Check-33</t>
+  </si>
+  <si>
+    <t>Veer_New-02</t>
+  </si>
+  <si>
+    <t>Veer_New-03</t>
+  </si>
+  <si>
+    <t>Test-Check-34</t>
+  </si>
+  <si>
+    <t>Test-Check-36</t>
+  </si>
+  <si>
+    <t>Test-Check-37</t>
+  </si>
+  <si>
+    <t>Test-Check-38</t>
   </si>
 </sst>
 </file>
@@ -478,7 +502,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F41"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
@@ -917,6 +941,278 @@
         <v>28</v>
       </c>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>